<commit_message>
com correção do svr
</commit_message>
<xml_diff>
--- a/seletor de Modelo/CIF_ERROS.xlsx
+++ b/seletor de Modelo/CIF_ERROS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amaral\Documents\Faculdade\tcc\seletor de Modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC06240E-C7D4-41EA-8858-3CC197302EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454494CA-C33D-4A42-8DDD-AEBED993E6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validation_rmse" sheetId="1" r:id="rId1"/>
@@ -762,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A58" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18188,7 +18188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S49" workbookViewId="0"/>
+    <sheetView topLeftCell="S49" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -26901,7 +26901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AL75"/>
   <sheetViews>
-    <sheetView topLeftCell="AA52" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>